<commit_message>
end of second day
</commit_message>
<xml_diff>
--- a/day2/sample.xlsx
+++ b/day2/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>apple</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>orange</t>
+  </si>
+  <si>
+    <t>sheet2</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -402,12 +405,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1020</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>